<commit_message>
change icecream names in xlsx
</commit_message>
<xml_diff>
--- a/ch17_tidyデータにしてみよう/ranking.xlsx
+++ b/ch17_tidyデータにしてみよう/ranking.xlsx
@@ -1,85 +1,92 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ma060\OneDrive\ドキュメント\book\r_rakuraku_book\ch17_tidyデータにしてみよう\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FDC23D-B40F-4803-B71C-4D049D76C47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t xml:space="preserve">ランキング</t>
-  </si>
-  <si>
-    <t xml:space="preserve">価格</t>
-  </si>
-  <si>
-    <t xml:space="preserve">今月(2021/12)のランキング</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1ヵ月前のランキング</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2ヵ月前のランキング</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3ヵ月前のランキング</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4ヵ月前のランキング</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5ヵ月前のランキング</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6ヵ月前のランキング</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7ヵ月前のランキング</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8ヵ月前のランキング</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9ヵ月前のランキング</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10ヵ月前のランキング</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11ヵ月前のランキング</t>
-  </si>
-  <si>
-    <t xml:space="preserve">チョコ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">抹茶</t>
-  </si>
-  <si>
-    <t xml:space="preserve">バニラ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ストロベリー</t>
-  </si>
-  <si>
-    <t xml:space="preserve">アズキ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">オレンジ</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="20">
+  <si>
+    <t>ランキング</t>
+  </si>
+  <si>
+    <t>価格</t>
+  </si>
+  <si>
+    <t>今月(2021/12)のランキング</t>
+  </si>
+  <si>
+    <t>1ヵ月前のランキング</t>
+  </si>
+  <si>
+    <t>2ヵ月前のランキング</t>
+  </si>
+  <si>
+    <t>3ヵ月前のランキング</t>
+  </si>
+  <si>
+    <t>4ヵ月前のランキング</t>
+  </si>
+  <si>
+    <t>5ヵ月前のランキング</t>
+  </si>
+  <si>
+    <t>6ヵ月前のランキング</t>
+  </si>
+  <si>
+    <t>7ヵ月前のランキング</t>
+  </si>
+  <si>
+    <t>8ヵ月前のランキング</t>
+  </si>
+  <si>
+    <t>9ヵ月前のランキング</t>
+  </si>
+  <si>
+    <t>10ヵ月前のランキング</t>
+  </si>
+  <si>
+    <t>11ヵ月前のランキング</t>
+  </si>
+  <si>
+    <t>チョコ</t>
+  </si>
+  <si>
+    <t>抹茶</t>
+  </si>
+  <si>
+    <t>バニラ</t>
+  </si>
+  <si>
+    <t>オレンジ</t>
+  </si>
+  <si>
+    <t>あずき</t>
+  </si>
+  <si>
+    <t>いちご</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -112,9 +119,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,14 +412,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,11 +465,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>800</v>
       </c>
       <c r="C2" t="s">
@@ -470,13 +488,13 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K2" t="s">
         <v>18</v>
@@ -491,39 +509,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>750</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
         <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
         <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L3" t="s">
         <v>15</v>
@@ -532,14 +550,14 @@
         <v>16</v>
       </c>
       <c r="N3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>900</v>
       </c>
       <c r="C4" t="s">
@@ -555,10 +573,10 @@
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
@@ -567,7 +585,7 @@
         <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L4" t="s">
         <v>14</v>
@@ -579,11 +597,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>890</v>
       </c>
       <c r="C5" t="s">
@@ -614,27 +632,27 @@
         <v>16</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="N5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>700</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -649,7 +667,7 @@
         <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
         <v>18</v>
@@ -658,17 +676,17 @@
         <v>15</v>
       </c>
       <c r="L6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>